<commit_message>
Random spreadsheet changes and got rtsc 3 compartment data
</commit_message>
<xml_diff>
--- a/AIC9parameters_RTSC_3comp.xlsx
+++ b/AIC9parameters_RTSC_3comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DA6FB1-75CB-45D1-946E-CFB51EBE2CC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0722B2-C19A-45C7-B593-65A36F7A41A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{C047B165-581C-4568-96D0-E1FF7B110487}"/>
   </bookViews>
@@ -387,123 +387,123 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2523.4646750613356</v>
+        <v>2449.3771339139662</v>
       </c>
       <c r="B1">
-        <v>1556.3325509160818</v>
+        <v>1583.5257250288973</v>
       </c>
       <c r="C1">
-        <v>1720.48614545192</v>
+        <v>1656.8653449771427</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2449.3771339139662</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>1583.5257250288973</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1656.8653449771427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2410.3949810358085</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>1638.4099719128481</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>1660.9951547017859</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2389.1784548155265</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>1595.8556395611924</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1625.2028737748544</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2370.3436748785252</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>1567.3377165411903</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1667.9900621380857</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2354.5589109541329</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>1895.1454140999226</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1886.0706153125413</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2340.0987397129452</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>1876.9544773212288</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1868.0912373037841</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2324.292942610286</v>
+        <v>0</v>
       </c>
       <c r="B8">
-        <v>1859.654584703236</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1850.837207813204</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2304.9013882843869</v>
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>1842.7878300956017</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>1833.749532510993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2278.1904748871916</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>1831.5301929676973</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1811.6113898358881</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2245.9442018545174</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>1816.482149322929</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>1790.19828541675</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>